<commit_message>
added latest manugacturing files, double checked BOM
</commit_message>
<xml_diff>
--- a/hardware/PCB/tstick-5gw-pro-USB-V2-pcb/tstick-5gw-pro-USB-V2-BOM.xlsx
+++ b/hardware/PCB/tstick-5gw-pro-USB-V2-pcb/tstick-5gw-pro-USB-V2-BOM.xlsx
@@ -362,7 +362,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -392,12 +392,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -451,11 +445,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -468,23 +462,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
 </styleSheet>
 </file>
 
@@ -496,7 +473,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -528,16 +505,16 @@
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>2659</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="0" t="s">
+      <c r="C2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -545,16 +522,16 @@
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" s="0" t="s">
+      <c r="C3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -562,33 +539,33 @@
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -596,33 +573,33 @@
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="0" t="s">
+      <c r="C6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="0" t="s">
+      <c r="C7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -630,16 +607,16 @@
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="0" t="s">
+      <c r="C8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="1" t="s">
         <v>31</v>
       </c>
     </row>
@@ -647,16 +624,16 @@
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="1" t="s">
         <v>34</v>
       </c>
     </row>
@@ -664,67 +641,67 @@
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D12" s="0" t="s">
+      <c r="C12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" s="0" t="s">
+      <c r="C13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" s="1" t="s">
         <v>49</v>
       </c>
     </row>
@@ -732,50 +709,50 @@
       <c r="A14" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D14" s="0" t="s">
+      <c r="C14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D15" s="0" t="s">
+      <c r="C15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D16" s="0" t="s">
+      <c r="C16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="E16" s="1" t="s">
         <v>57</v>
       </c>
     </row>
@@ -783,16 +760,16 @@
       <c r="A17" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C17" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="E17" s="1" t="s">
         <v>63</v>
       </c>
     </row>
@@ -800,16 +777,16 @@
       <c r="A18" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="C18" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="E18" s="1" t="s">
         <v>66</v>
       </c>
     </row>
@@ -817,16 +794,16 @@
       <c r="A19" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D19" s="0" t="s">
+      <c r="C19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="E19" s="1" t="s">
         <v>69</v>
       </c>
     </row>
@@ -834,16 +811,16 @@
       <c r="A20" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D20" s="0" t="s">
+      <c r="C20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="E20" s="1" t="s">
         <v>72</v>
       </c>
     </row>
@@ -851,16 +828,16 @@
       <c r="A21" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="0" t="n">
+      <c r="C21" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="E21" s="1" t="s">
         <v>75</v>
       </c>
     </row>
@@ -868,16 +845,16 @@
       <c r="A22" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C22" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D22" s="0" t="s">
+      <c r="C22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="E22" s="1" t="s">
         <v>78</v>
       </c>
     </row>
@@ -885,16 +862,16 @@
       <c r="A23" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D23" s="0" t="s">
+      <c r="C23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="E23" s="1" t="s">
         <v>81</v>
       </c>
     </row>
@@ -902,16 +879,16 @@
       <c r="A24" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C24" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D24" s="0" t="s">
+      <c r="C24" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E24" s="0" t="s">
+      <c r="E24" s="1" t="s">
         <v>84</v>
       </c>
     </row>
@@ -919,16 +896,16 @@
       <c r="A25" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C25" s="0" t="n">
+      <c r="C25" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="E25" s="1" t="s">
         <v>87</v>
       </c>
     </row>
@@ -936,16 +913,16 @@
       <c r="A26" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="C26" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E26" s="0" t="s">
+      <c r="E26" s="1" t="s">
         <v>90</v>
       </c>
     </row>
@@ -953,16 +930,16 @@
       <c r="A27" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C27" s="0" t="n">
+      <c r="C27" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="D27" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E27" s="0" t="s">
+      <c r="E27" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -970,16 +947,16 @@
       <c r="A28" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C28" s="0" t="n">
+      <c r="C28" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D28" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E28" s="0" t="s">
+      <c r="E28" s="1" t="s">
         <v>97</v>
       </c>
     </row>
@@ -987,16 +964,16 @@
       <c r="A29" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C29" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D29" s="0" t="s">
+      <c r="C29" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E29" s="0" t="s">
+      <c r="E29" s="1" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1004,16 +981,16 @@
       <c r="A30" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C30" s="0" t="n">
+      <c r="C30" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E30" s="0" t="s">
+      <c r="E30" s="1" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1021,16 +998,16 @@
       <c r="A31" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C31" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D31" s="0" t="s">
+      <c r="C31" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E31" s="0" t="s">
+      <c r="E31" s="1" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1038,16 +1015,16 @@
       <c r="A32" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C32" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D32" s="0" t="s">
+      <c r="C32" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E32" s="0" t="s">
+      <c r="E32" s="1" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added updated bill of materials and manufacturing files
</commit_message>
<xml_diff>
--- a/hardware/PCB/tstick-5gw-pro-USB-V2-pcb/tstick-5gw-pro-USB-V2-BOM.xlsx
+++ b/hardware/PCB/tstick-5gw-pro-USB-V2-pcb/tstick-5gw-pro-USB-V2-BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="112">
   <si>
     <t xml:space="preserve">Manufacturer</t>
   </si>
@@ -160,16 +160,16 @@
     <t xml:space="preserve">QFN-20 Battery Management ICs ROHS</t>
   </si>
   <si>
-    <t xml:space="preserve">Nexperia USA Inc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PESD5Z3.3,115</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18V Clamp 20A (8/20µs) Ipp Tvs Diode Surface Mount SOD-523</t>
+    <t xml:space="preserve">STMicroelectronics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USBLC6-2P6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17V Clamp 5A (8/20µs) Ipp Tvs Diode Surface Mount SOT-666</t>
   </si>
   <si>
     <t xml:space="preserve">Ohmite</t>
@@ -193,7 +193,7 @@
     <t xml:space="preserve">U4</t>
   </si>
   <si>
-    <t xml:space="preserve">Linear Voltage Regulator IC Positive Fixed 1 Output 700mA 4-XDFN (1x1)</t>
+    <t xml:space="preserve">Linear Voltage Regulator IC Positive Fixed 1 Output 700mA 4-XDFN (1x1), 1.8V</t>
   </si>
   <si>
     <t xml:space="preserve">NCP167AMX330TBG</t>
@@ -202,6 +202,9 @@
     <t xml:space="preserve">U3</t>
   </si>
   <si>
+    <t xml:space="preserve">Linear Voltage Regulator IC Positive Fixed 1 Output 700mA 4-XDFN (1x1), 3.3V</t>
+  </si>
+  <si>
     <t xml:space="preserve">Panasonic Electronic Components</t>
   </si>
   <si>
@@ -238,7 +241,7 @@
     <t xml:space="preserve">R20</t>
   </si>
   <si>
-    <t xml:space="preserve">RES SMD 2K OHM 1% 1/20W 0201</t>
+    <t xml:space="preserve">2 kOhms ±1% 0.05W, 1/20W Chip Resistor 0201 (0603 Metric) Thick Film</t>
   </si>
   <si>
     <t xml:space="preserve">ERJ-1GNF2201C</t>
@@ -301,7 +304,7 @@
     <t xml:space="preserve">CL03A104KP3NNNC</t>
   </si>
   <si>
-    <t xml:space="preserve">C1, C6, C7, C13</t>
+    <t xml:space="preserve">C1, C6, C7, C13, C15</t>
   </si>
   <si>
     <t xml:space="preserve">0.1 µF ±10% 10V Ceramic Capacitor X5R 0201 (0603 Metric)</t>
@@ -473,7 +476,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -753,279 +756,279 @@
         <v>59</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>4</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>6</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>4</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C28" s="1" t="n">
         <v>6</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C30" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added up to date manufacturing files
</commit_message>
<xml_diff>
--- a/hardware/PCB/tstick-5gw-pro-USB-V2-pcb/tstick-5gw-pro-USB-V2-BOM.xlsx
+++ b/hardware/PCB/tstick-5gw-pro-USB-V2-pcb/tstick-5gw-pro-USB-V2-BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="114">
   <si>
     <t xml:space="preserve">Manufacturer</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">Description Value Pkg</t>
   </si>
   <si>
+    <t xml:space="preserve">Note</t>
+  </si>
+  <si>
     <t xml:space="preserve">Adafruit Industries LLC</t>
   </si>
   <si>
@@ -104,6 +107,12 @@
   </si>
   <si>
     <t xml:space="preserve">USB-C (USB TYPE-C) USB 2.0 Receptacle Connector 24 (16+8 Dummy) Position Surface Mount, Right Angle; Through Hole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The products sealed in moisture barrier bags (MBB) should be stored in a non-condensing atmospheric
+environment of &lt; 40 °C and 90%RH. The module is rated at the moisture sensitivity level (MSL) of 3.
+After unpacking, the module must be soldered within 168 hours with the factory conditions 25±5 °C and
+60%RH. If the above conditions are not met, the module needs to be baked.</t>
   </si>
   <si>
     <t xml:space="preserve">JST Sales America Inc.</t>
@@ -439,7 +448,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -452,8 +461,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -473,10 +490,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E60" activeCellId="0" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -503,10 +520,13 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>2659</v>
@@ -515,520 +535,523 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>12</v>
+      <c r="A4" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>3</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>4</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>6</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>4</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C28" s="1" t="n">
         <v>6</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C30" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reduced size of esp32 pcb to 1x2.35 inch, used ssmaller neopixel, updated BOM
</commit_message>
<xml_diff>
--- a/hardware/PCB/tstick-5gw-pro-USB-V2-pcb/tstick-5gw-pro-USB-V2-BOM.xlsx
+++ b/hardware/PCB/tstick-5gw-pro-USB-V2-pcb/tstick-5gw-pro-USB-V2-BOM.xlsx
@@ -46,7 +46,10 @@
     <t xml:space="preserve">PWLED1</t>
   </si>
   <si>
-    <t xml:space="preserve">Addressable Lighting Neopixel 10 LED Discrete Serial (Shift Register) Red, Green, Blue (RGB) 3.50mm L x 3.50mm W</t>
+    <t xml:space="preserve">Addressable Lighting Neopixel 10 LED Discrete Red, Green, Blue (RGB) 1.50mm L x 1.50mm W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comes in reel of 10</t>
   </si>
   <si>
     <t xml:space="preserve">Analog Devices Inc./Maxim Integrated</t>
@@ -109,12 +112,6 @@
     <t xml:space="preserve">USB-C (USB TYPE-C) USB 2.0 Receptacle Connector 24 (16+8 Dummy) Position Surface Mount, Right Angle; Through Hole</t>
   </si>
   <si>
-    <t xml:space="preserve">The products sealed in moisture barrier bags (MBB) should be stored in a non-condensing atmospheric
-environment of &lt; 40 °C and 90%RH. The module is rated at the moisture sensitivity level (MSL) of 3.
-After unpacking, the module must be soldered within 168 hours with the factory conditions 25±5 °C and
-60%RH. If the above conditions are not met, the module needs to be baked.</t>
-  </si>
-  <si>
     <t xml:space="preserve">JST Sales America Inc.</t>
   </si>
   <si>
@@ -274,7 +271,7 @@
     <t xml:space="preserve">ERJ-1GNF3000C</t>
   </si>
   <si>
-    <t xml:space="preserve">R13</t>
+    <t xml:space="preserve">R8</t>
   </si>
   <si>
     <t xml:space="preserve">300 Ohms ±1% 0.05W, 1/20W Chip Resistor 0201 (0603 Metric) Thick Film</t>
@@ -448,7 +445,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -461,15 +458,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -490,10 +483,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E60" activeCellId="0" sqref="E60"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -520,7 +513,7 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -529,7 +522,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>2659</v>
+        <v>4492</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>1</v>
@@ -540,94 +533,95 @@
       <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F2" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>13</v>
+      <c r="A4" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="5" t="s">
         <v>29</v>
       </c>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
@@ -1054,6 +1048,7 @@
         <v>113</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
updated pcb BOM, switched buttons to smaller 3x2mm buttons
</commit_message>
<xml_diff>
--- a/hardware/PCB/tstick-5gw-pro-USB-V2-pcb/tstick-5gw-pro-USB-V2-BOM.xlsx
+++ b/hardware/PCB/tstick-5gw-pro-USB-V2-pcb/tstick-5gw-pro-USB-V2-BOM.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Github\T-Stick\hardware\PCB\tstick-5gw-pro-USB-V2-pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2707DD-0680-496B-8B1E-64AE7785E2D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588CDFF4-5A7D-4652-A3B6-102EC183054B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tstick-5gw-pro-USB-BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -81,12 +81,6 @@
     <t>N-Channel 50 V 220mA (Ta) 350mW (Ta) Surface Mount SOT-23</t>
   </si>
   <si>
-    <t>C&amp;K</t>
-  </si>
-  <si>
-    <t>PTS810 SJM 250 SMTR LFS</t>
-  </si>
-  <si>
     <t>Tactile Switch SPST-NO Top Actuated Surface Mount</t>
   </si>
   <si>
@@ -367,6 +361,12 @@
   </si>
   <si>
     <t>B2B-PH-SM4-TB</t>
+  </si>
+  <si>
+    <t>B3U-1000P</t>
+  </si>
+  <si>
+    <t>Omron Electronics Inc-EMC Div</t>
   </si>
 </sst>
 </file>
@@ -733,7 +733,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,479 +820,479 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>112</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" t="s">
+      <c r="E6" t="s">
         <v>22</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
         <v>25</v>
       </c>
-      <c r="B7" t="s">
+      <c r="E7" t="s">
         <v>26</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" t="s">
-        <v>28</v>
       </c>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s">
         <v>29</v>
-      </c>
-      <c r="B9" t="s">
-        <v>113</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C11">
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
         <v>40</v>
       </c>
-      <c r="B12" t="s">
+      <c r="E12" t="s">
         <v>41</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
         <v>48</v>
       </c>
-      <c r="B13" t="s">
+      <c r="E13" t="s">
         <v>49</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" t="s">
         <v>56</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
         <v>52</v>
       </c>
-      <c r="B15" t="s">
+      <c r="E15" t="s">
         <v>53</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C16">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" t="s">
         <v>66</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C19">
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" t="s">
         <v>78</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>79</v>
-      </c>
-      <c r="E20" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C21">
         <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" t="s">
         <v>75</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>76</v>
-      </c>
-      <c r="E22" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" t="s">
         <v>81</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>82</v>
-      </c>
-      <c r="E23" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" t="s">
         <v>69</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
-        <v>70</v>
-      </c>
-      <c r="E24" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C25">
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C26">
         <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B27" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>96</v>
+      </c>
+      <c r="E27" t="s">
         <v>97</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
-        <v>98</v>
-      </c>
-      <c r="E27" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B28" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C28">
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C29">
         <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E29" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>102</v>
+      </c>
+      <c r="E30" t="s">
         <v>103</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30" t="s">
-        <v>104</v>
-      </c>
-      <c r="E30" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
         <v>44</v>
       </c>
-      <c r="B31" t="s">
+      <c r="E31" t="s">
         <v>45</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31" t="s">
-        <v>46</v>
-      </c>
-      <c r="E31" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
         <v>106</v>
       </c>
-      <c r="B32" t="s">
+      <c r="E32" t="s">
         <v>107</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32" t="s">
-        <v>108</v>
-      </c>
-      <c r="E32" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated board flash size, added button interrupt, removed serial print
</commit_message>
<xml_diff>
--- a/hardware/PCB/tstick-5gw-pro-USB-V2-pcb/tstick-5gw-pro-USB-V2-BOM.xlsx
+++ b/hardware/PCB/tstick-5gw-pro-USB-V2-pcb/tstick-5gw-pro-USB-V2-BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Github\T-Stick\hardware\PCB\tstick-5gw-pro-USB-V2-pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588CDFF4-5A7D-4652-A3B6-102EC183054B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A5878F-0E69-4F86-85F9-065BE8411A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3000" yWindow="690" windowWidth="21600" windowHeight="12735" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tstick-5gw-pro-USB-BOM" sheetId="1" r:id="rId1"/>
@@ -213,9 +213,6 @@
     <t>ERJ-1GNF1002C</t>
   </si>
   <si>
-    <t>R5, R12</t>
-  </si>
-  <si>
     <t>10 kOhms ±1% 0.05W, 1/20W Chip Resistor 0201 (0603 Metric) Thick Film</t>
   </si>
   <si>
@@ -285,9 +282,6 @@
     <t>ERT-JZEG103FA</t>
   </si>
   <si>
-    <t>TH1, TH2</t>
-  </si>
-  <si>
     <t>NTC Thermistor 10k 0201 (0603 Metric)</t>
   </si>
   <si>
@@ -367,6 +361,12 @@
   </si>
   <si>
     <t>Omron Electronics Inc-EMC Div</t>
+  </si>
+  <si>
+    <t>R5, R9 R12</t>
+  </si>
+  <si>
+    <t>TH1</t>
   </si>
 </sst>
 </file>
@@ -732,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,16 +820,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E5" t="s">
         <v>18</v>
@@ -881,7 +881,7 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E8" t="s">
         <v>31</v>
@@ -892,7 +892,7 @@
         <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -915,7 +915,7 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E10" t="s">
         <v>33</v>
@@ -1028,16 +1028,16 @@
         <v>57</v>
       </c>
       <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
         <v>64</v>
       </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>65</v>
-      </c>
-      <c r="E17" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1048,13 +1048,13 @@
         <v>61</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D18" t="s">
+        <v>112</v>
+      </c>
+      <c r="E18" t="s">
         <v>62</v>
-      </c>
-      <c r="E18" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1062,16 +1062,16 @@
         <v>57</v>
       </c>
       <c r="B19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C19">
         <v>2</v>
       </c>
       <c r="D19" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" t="s">
         <v>83</v>
-      </c>
-      <c r="E19" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1079,16 +1079,16 @@
         <v>57</v>
       </c>
       <c r="B20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
         <v>76</v>
       </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>77</v>
-      </c>
-      <c r="E20" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1096,16 +1096,16 @@
         <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C21">
         <v>6</v>
       </c>
       <c r="D21" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" t="s">
         <v>71</v>
-      </c>
-      <c r="E21" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1113,16 +1113,16 @@
         <v>57</v>
       </c>
       <c r="B22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
         <v>73</v>
       </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>74</v>
-      </c>
-      <c r="E22" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1130,16 +1130,16 @@
         <v>57</v>
       </c>
       <c r="B23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
         <v>79</v>
       </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>80</v>
-      </c>
-      <c r="E23" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1147,16 +1147,16 @@
         <v>57</v>
       </c>
       <c r="B24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
         <v>67</v>
       </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>68</v>
-      </c>
-      <c r="E24" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1164,101 +1164,101 @@
         <v>57</v>
       </c>
       <c r="B25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>113</v>
+      </c>
+      <c r="E25" t="s">
         <v>85</v>
-      </c>
-      <c r="C25">
-        <v>2</v>
-      </c>
-      <c r="D25" t="s">
-        <v>86</v>
-      </c>
-      <c r="E25" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B26" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C26">
         <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B27" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>94</v>
+      </c>
+      <c r="E27" t="s">
         <v>95</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
-        <v>96</v>
-      </c>
-      <c r="E27" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B28" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C28">
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E28" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B29" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C29">
         <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B30" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>100</v>
+      </c>
+      <c r="E30" t="s">
         <v>101</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30" t="s">
-        <v>102</v>
-      </c>
-      <c r="E30" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1280,19 +1280,19 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" t="s">
+        <v>103</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
         <v>104</v>
       </c>
-      <c r="B32" t="s">
+      <c r="E32" t="s">
         <v>105</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32" t="s">
-        <v>106</v>
-      </c>
-      <c r="E32" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed some LED code, updated schematic, removed choke resistor from both board and BOM
</commit_message>
<xml_diff>
--- a/hardware/PCB/tstick-5gw-pro-USB-V2-pcb/tstick-5gw-pro-USB-V2-BOM.xlsx
+++ b/hardware/PCB/tstick-5gw-pro-USB-V2-pcb/tstick-5gw-pro-USB-V2-BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Github\T-Stick\hardware\PCB\tstick-5gw-pro-USB-V2-pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A5878F-0E69-4F86-85F9-065BE8411A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD1C3E7-4E45-43DE-87AA-847FE47C4955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="690" windowWidth="21600" windowHeight="12735" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="111">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -250,15 +250,6 @@
   </si>
   <si>
     <t>24.9 kOhms ±1% 0.05W, 1/20W Chip Resistor 0201 (0603 Metric) Thick Film</t>
-  </si>
-  <si>
-    <t>ERJ-1GNF3000C</t>
-  </si>
-  <si>
-    <t>R8</t>
-  </si>
-  <si>
-    <t>300 Ohms ±1% 0.05W, 1/20W Chip Resistor 0201 (0603 Metric) Thick Film</t>
   </si>
   <si>
     <t>ERJ-1GNF3303C</t>
@@ -730,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,16 +811,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E5" t="s">
         <v>18</v>
@@ -881,7 +872,7 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E8" t="s">
         <v>31</v>
@@ -892,7 +883,7 @@
         <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -915,7 +906,7 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E10" t="s">
         <v>33</v>
@@ -1051,7 +1042,7 @@
         <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E18" t="s">
         <v>62</v>
@@ -1062,16 +1053,16 @@
         <v>57</v>
       </c>
       <c r="B19" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C19">
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E19" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1079,16 +1070,16 @@
         <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E20" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1096,16 +1087,16 @@
         <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C21">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E21" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1113,16 +1104,16 @@
         <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E22" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1130,16 +1121,16 @@
         <v>57</v>
       </c>
       <c r="B23" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="E23" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1147,61 +1138,61 @@
         <v>57</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
       <c r="E24" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="B25" t="s">
         <v>84</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="E25" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B26" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C26">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E26" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B27" t="s">
         <v>93</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D27" t="s">
         <v>94</v>
@@ -1212,92 +1203,75 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B28" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="E28" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B29" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C29">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="E29" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>86</v>
+        <v>42</v>
       </c>
       <c r="B30" t="s">
-        <v>99</v>
+        <v>43</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>100</v>
+        <v>44</v>
       </c>
       <c r="E30" t="s">
-        <v>101</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>99</v>
       </c>
       <c r="B31" t="s">
-        <v>43</v>
+        <v>100</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>44</v>
+        <v>101</v>
       </c>
       <c r="E31" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
         <v>102</v>
       </c>
-      <c r="B32" t="s">
-        <v>103</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32" t="s">
-        <v>104</v>
-      </c>
-      <c r="E32" t="s">
-        <v>105</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F32">
-    <sortCondition ref="A1:A32"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F31">
+    <sortCondition ref="A1:A31"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
increased PCB board length, updated LEDs
</commit_message>
<xml_diff>
--- a/hardware/PCB/tstick-5gw-pro-USB-V2-pcb/tstick-5gw-pro-USB-V2-BOM.xlsx
+++ b/hardware/PCB/tstick-5gw-pro-USB-V2-pcb/tstick-5gw-pro-USB-V2-BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aniyo\Documents\GitHub\T-Stick\hardware\PCB\tstick-5gw-pro-USB-V2-pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38184B16-3357-4FB6-9A36-A929BE5C23B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B83383-A030-4F77-9892-F139F2A76E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tstick-5gw-pro-USB-BOM" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="121">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -159,24 +159,12 @@
     <t>Green 570nm LED Indication - Discrete 2.1V 0402 (1005 Metric)</t>
   </si>
   <si>
-    <t>APHHS1005QBC/D</t>
-  </si>
-  <si>
     <t>STATLED1</t>
   </si>
   <si>
-    <t>Blue 465nm LED Indication - Discrete 3.3V 0402 (1005 Metric)</t>
-  </si>
-  <si>
-    <t>APHHS1005SECK</t>
-  </si>
-  <si>
     <t>STATLED2</t>
   </si>
   <si>
-    <t>Orange 601nm LED Indication - Discrete 2.1V 0402 (1005 Metric)</t>
-  </si>
-  <si>
     <t>Microchip Technology</t>
   </si>
   <si>
@@ -385,6 +373,21 @@
   </si>
   <si>
     <t>0.1 µF ±10% 16V Ceramic Capacitor X7R 0402 (1005 Metric)</t>
+  </si>
+  <si>
+    <t>IN-S42BT5B</t>
+  </si>
+  <si>
+    <t>Inolux</t>
+  </si>
+  <si>
+    <t>Blue 467nm LED Indication - Discrete 2.9V 0402 (1005 Metric)</t>
+  </si>
+  <si>
+    <t>IN-S42BT5A</t>
+  </si>
+  <si>
+    <t>Amber 605nm LED Indication - Discrete 2V 0402 (1005 Metric)</t>
   </si>
 </sst>
 </file>
@@ -750,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,7 +876,7 @@
         <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -882,7 +885,7 @@
         <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -955,87 +958,87 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>117</v>
       </c>
       <c r="B12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
         <v>44</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>45</v>
-      </c>
       <c r="E12" t="s">
-        <v>46</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>117</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>119</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E13" t="s">
-        <v>49</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E14" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B15" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E15" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E16" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1057,291 +1060,291 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E18" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" t="s">
         <v>58</v>
       </c>
-      <c r="B19" t="s">
-        <v>62</v>
-      </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E19" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C20">
         <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E20" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B21" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E21" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C22">
         <v>3</v>
       </c>
       <c r="D22" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E22" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C23">
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E23" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C24">
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E24" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
         <v>65</v>
       </c>
-      <c r="B25" t="s">
-        <v>89</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
-        <v>69</v>
-      </c>
       <c r="E25" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E26" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B27" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E27" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E28" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B29" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C29">
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E29" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B30" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C30">
         <v>2</v>
       </c>
       <c r="D30" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E30" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C31">
         <v>6</v>
       </c>
       <c r="D31" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E31" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B32" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C32">
         <v>2</v>
       </c>
       <c r="D32" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E32" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B33" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E33" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B34" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C34">
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E34" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>